<commit_message>
优化 JxlsPlusUtils 工具类，默认注入 stringUtils 和 dateUtils 两个工具类
</commit_message>
<xml_diff>
--- a/src/test/resources/each_template.xlsx
+++ b/src/test/resources/each_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace_tzg\jxls-plus\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492ED538-D053-46E3-9649-A39FF433ED54}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39797965-1644-4269-9ED2-B7A8FDEB757B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>jx:area(lastCell="F5")</t>
+          <t>jx:area(lastCell="G7")</t>
         </r>
       </text>
     </comment>
@@ -59,7 +59,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>jx:each(items="employees" var="emp" lastCell="F5")</t>
+          <t>jx:each(items="employees" var="emp" lastCell="G6")</t>
         </r>
       </text>
     </comment>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>员工信息</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -114,11 +114,30 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>${emp.lastLoginDate}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>最后登录时间</t>
+    <t>入职时间</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>奖金</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${emp.bonus}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>办公室</t>
+  </si>
+  <si>
+    <t>${off.officeName}（${off.officeCode}）</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>合计</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${dateUtils.formatUTC(emp.hiredate,"yyyy-MM-dd")}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -126,8 +145,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd;@"/>
+  <numFmts count="3">
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="177" formatCode="[$¥-804]#,##0.00_);[Red]\([$¥-804]#,##0.00\)"/>
+    <numFmt numFmtId="178" formatCode="0;[Red]0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -191,7 +212,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -214,11 +235,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -226,20 +260,41 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -521,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
@@ -534,80 +589,109 @@
     <col min="3" max="3" width="7.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.875" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="1"/>
+    <col min="6" max="6" width="14.25" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:7" ht="63" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>11</v>
+      <c r="F5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+    <row r="6" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="7">
+        <f>SUM(G5)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:F2"/>
+  <mergeCells count="2">
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="E6:G6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>